<commit_message>
se agrega R project
</commit_message>
<xml_diff>
--- a/results/enge/enge_y_total.xlsx
+++ b/results/enge/enge_y_total.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P29"/>
+  <dimension ref="A1:S29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,7 +451,7 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>productividad_ipi_enge_index_1</t>
+          <t>productividad_enge_index_1</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
@@ -501,10 +501,25 @@
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
+          <t>productividad_tot_level</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>productividad_enge_level</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>brecha_productividad_enge_tot_level</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
           <t>peso_vab_enge</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>peso_emp_enge</t>
         </is>
@@ -556,9 +571,18 @@
         <v>0.7593361020635817</v>
       </c>
       <c r="O2" t="n">
+        <v>0.04304377887543848</v>
+      </c>
+      <c r="P2" t="n">
+        <v>0.1180673020322136</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>2.742958567227117</v>
+      </c>
+      <c r="R2" t="n">
         <v>0.3775669637942825</v>
       </c>
-      <c r="P2" t="n">
+      <c r="S2" t="n">
         <v>0.1376495322625192</v>
       </c>
     </row>
@@ -608,9 +632,18 @@
         <v>0.8423616676040163</v>
       </c>
       <c r="O3" t="n">
+        <v>0.04880858172414023</v>
+      </c>
+      <c r="P3" t="n">
+        <v>0.1354902191704453</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>2.775950752599583</v>
+      </c>
+      <c r="R3" t="n">
         <v>0.3941197999292144</v>
       </c>
-      <c r="P3" t="n">
+      <c r="S3" t="n">
         <v>0.1419765100516047</v>
       </c>
     </row>
@@ -660,9 +693,18 @@
         <v>0.8674743887405572</v>
       </c>
       <c r="O4" t="n">
+        <v>0.0492551047037967</v>
+      </c>
+      <c r="P4" t="n">
+        <v>0.1272343016830642</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>2.58316985514918</v>
+      </c>
+      <c r="R4" t="n">
         <v>0.3875027923709867</v>
       </c>
-      <c r="P4" t="n">
+      <c r="S4" t="n">
         <v>0.1500105738685961</v>
       </c>
     </row>
@@ -712,9 +754,18 @@
         <v>0.967144619540799</v>
       </c>
       <c r="O5" t="n">
+        <v>0.05439834344477179</v>
+      </c>
+      <c r="P5" t="n">
+        <v>0.1375438130452666</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>2.528455911252311</v>
+      </c>
+      <c r="R5" t="n">
         <v>0.3826609358685141</v>
       </c>
-      <c r="P5" t="n">
+      <c r="S5" t="n">
         <v>0.1513417474141312</v>
       </c>
     </row>
@@ -764,9 +815,18 @@
         <v>1</v>
       </c>
       <c r="O6" t="n">
+        <v>0.05715512483064726</v>
+      </c>
+      <c r="P6" t="n">
+        <v>0.1477945882774631</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>2.585850152814536</v>
+      </c>
+      <c r="R6" t="n">
         <v>0.3929093362803455</v>
       </c>
-      <c r="P6" t="n">
+      <c r="S6" t="n">
         <v>0.1519459029181131</v>
       </c>
     </row>
@@ -816,9 +876,18 @@
         <v>0.9341764799503322</v>
       </c>
       <c r="O7" t="n">
+        <v>0.05487749065859163</v>
+      </c>
+      <c r="P7" t="n">
+        <v>0.1542553995581563</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>2.81090475724961</v>
+      </c>
+      <c r="R7" t="n">
         <v>0.4034773671121105</v>
       </c>
-      <c r="P7" t="n">
+      <c r="S7" t="n">
         <v>0.1435400349554716</v>
       </c>
     </row>
@@ -868,9 +937,18 @@
         <v>0.9101358570389435</v>
       </c>
       <c r="O8" t="n">
+        <v>0.05286027224267655</v>
+      </c>
+      <c r="P8" t="n">
+        <v>0.1490723924546326</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>2.820121541755504</v>
+      </c>
+      <c r="R8" t="n">
         <v>0.3939365565247019</v>
       </c>
-      <c r="P8" t="n">
+      <c r="S8" t="n">
         <v>0.1396877938386583</v>
       </c>
     </row>
@@ -920,9 +998,18 @@
         <v>0.8356558220032069</v>
       </c>
       <c r="O9" t="n">
+        <v>0.05202265186443492</v>
+      </c>
+      <c r="P9" t="n">
+        <v>0.1622246747026341</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>3.118346890992276</v>
+      </c>
+      <c r="R9" t="n">
         <v>0.4343006166883199</v>
       </c>
-      <c r="P9" t="n">
+      <c r="S9" t="n">
         <v>0.1392727082233378</v>
       </c>
     </row>
@@ -972,9 +1059,18 @@
         <v>0.7555008925758326</v>
       </c>
       <c r="O10" t="n">
+        <v>0.04828995604331608</v>
+      </c>
+      <c r="P10" t="n">
+        <v>0.1610089082777418</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>3.334211116972581</v>
+      </c>
+      <c r="R10" t="n">
         <v>0.4453849335967244</v>
       </c>
-      <c r="P10" t="n">
+      <c r="S10" t="n">
         <v>0.1335803036974839</v>
       </c>
     </row>
@@ -1024,9 +1120,18 @@
         <v>0.4925947998598897</v>
       </c>
       <c r="O11" t="n">
+        <v>0.04320617777713606</v>
+      </c>
+      <c r="P11" t="n">
+        <v>0.1977569747057514</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>4.577053210441607</v>
+      </c>
+      <c r="R11" t="n">
         <v>0.5940694637962298</v>
       </c>
-      <c r="P11" t="n">
+      <c r="S11" t="n">
         <v>0.1297929992251308</v>
       </c>
     </row>
@@ -1076,9 +1181,18 @@
         <v>0.5598395744318643</v>
       </c>
       <c r="O12" t="n">
+        <v>0.04414878162373259</v>
+      </c>
+      <c r="P12" t="n">
+        <v>0.2076309449113102</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>4.702982444247029</v>
+      </c>
+      <c r="R12" t="n">
         <v>0.5408286133816917</v>
       </c>
-      <c r="P12" t="n">
+      <c r="S12" t="n">
         <v>0.1149969449797258</v>
       </c>
     </row>
@@ -1128,9 +1242,18 @@
         <v>0.5686176341524102</v>
       </c>
       <c r="O13" t="n">
+        <v>0.04771119628556293</v>
+      </c>
+      <c r="P13" t="n">
+        <v>0.2275962511015319</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>4.770290179674261</v>
+      </c>
+      <c r="R13" t="n">
         <v>0.5707149543900899</v>
       </c>
-      <c r="P13" t="n">
+      <c r="S13" t="n">
         <v>0.1196394627777258</v>
       </c>
     </row>
@@ -1180,9 +1303,18 @@
         <v>0.5562676205545934</v>
       </c>
       <c r="O14" t="n">
+        <v>0.04694017916854153</v>
+      </c>
+      <c r="P14" t="n">
+        <v>0.2285720660474743</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>4.869433182748889</v>
+      </c>
+      <c r="R14" t="n">
         <v>0.572097217740351</v>
       </c>
-      <c r="P14" t="n">
+      <c r="S14" t="n">
         <v>0.117487435656195</v>
       </c>
     </row>
@@ -1232,9 +1364,18 @@
         <v>0.5857026777702944</v>
       </c>
       <c r="O15" t="n">
+        <v>0.0485698934869174</v>
+      </c>
+      <c r="P15" t="n">
+        <v>0.2319246168519907</v>
+      </c>
+      <c r="Q15" t="n">
+        <v>4.775069496795604</v>
+      </c>
+      <c r="R15" t="n">
         <v>0.5649826354889843</v>
       </c>
-      <c r="P15" t="n">
+      <c r="S15" t="n">
         <v>0.1183192487288669</v>
       </c>
     </row>
@@ -1284,9 +1425,18 @@
         <v>0.5949857663953879</v>
       </c>
       <c r="O16" t="n">
+        <v>0.05283084474046141</v>
+      </c>
+      <c r="P16" t="n">
+        <v>0.2489664574161446</v>
+      </c>
+      <c r="Q16" t="n">
+        <v>4.712520851014697</v>
+      </c>
+      <c r="R16" t="n">
         <v>0.5976468012724856</v>
       </c>
-      <c r="P16" t="n">
+      <c r="S16" t="n">
         <v>0.1268210412573136</v>
       </c>
     </row>
@@ -1336,9 +1486,18 @@
         <v>0.5763611239471179</v>
       </c>
       <c r="O17" t="n">
+        <v>0.05226348778732503</v>
+      </c>
+      <c r="P17" t="n">
+        <v>0.2500005338233884</v>
+      </c>
+      <c r="Q17" t="n">
+        <v>4.783464410961465</v>
+      </c>
+      <c r="R17" t="n">
         <v>0.6059444463212876</v>
       </c>
-      <c r="P17" t="n">
+      <c r="S17" t="n">
         <v>0.1266748101925346</v>
       </c>
     </row>
@@ -1388,9 +1547,18 @@
         <v>0.5674087394180646</v>
       </c>
       <c r="O18" t="n">
+        <v>0.04825279851919508</v>
+      </c>
+      <c r="P18" t="n">
+        <v>0.2279484594432366</v>
+      </c>
+      <c r="Q18" t="n">
+        <v>4.724046406397718</v>
+      </c>
+      <c r="R18" t="n">
         <v>0.5777118708289191</v>
       </c>
-      <c r="P18" t="n">
+      <c r="S18" t="n">
         <v>0.1222917433762994</v>
       </c>
     </row>
@@ -1440,9 +1608,18 @@
         <v>0.7226473903798223</v>
       </c>
       <c r="O19" t="n">
+        <v>0.05829695560972845</v>
+      </c>
+      <c r="P19" t="n">
+        <v>0.238833472613862</v>
+      </c>
+      <c r="Q19" t="n">
+        <v>4.096842967456881</v>
+      </c>
+      <c r="R19" t="n">
         <v>0.5624458989007148</v>
       </c>
-      <c r="P19" t="n">
+      <c r="S19" t="n">
         <v>0.1372876391329818</v>
       </c>
     </row>
@@ -1492,9 +1669,18 @@
         <v>0.7351089860794459</v>
       </c>
       <c r="O20" t="n">
+        <v>0.05904918268858964</v>
+      </c>
+      <c r="P20" t="n">
+        <v>0.2434690385890328</v>
+      </c>
+      <c r="Q20" t="n">
+        <v>4.123156790721839</v>
+      </c>
+      <c r="R20" t="n">
         <v>0.5597971816002848</v>
       </c>
-      <c r="P20" t="n">
+      <c r="S20" t="n">
         <v>0.1357690745256092</v>
       </c>
     </row>
@@ -1544,9 +1730,18 @@
         <v>0.6311406239898477</v>
       </c>
       <c r="O21" t="n">
+        <v>0.05452291288786801</v>
+      </c>
+      <c r="P21" t="n">
+        <v>0.2402537549648996</v>
+      </c>
+      <c r="Q21" t="n">
+        <v>4.406473209877951</v>
+      </c>
+      <c r="R21" t="n">
         <v>0.5897677785828782</v>
       </c>
-      <c r="P21" t="n">
+      <c r="S21" t="n">
         <v>0.1338412264168091</v>
       </c>
     </row>
@@ -1596,9 +1791,18 @@
         <v>0.6420574868923955</v>
       </c>
       <c r="O22" t="n">
+        <v>0.05561776560386605</v>
+      </c>
+      <c r="P22" t="n">
+        <v>0.2376058822943495</v>
+      </c>
+      <c r="Q22" t="n">
+        <v>4.272122040764494</v>
+      </c>
+      <c r="R22" t="n">
         <v>0.5932615593695892</v>
       </c>
-      <c r="P22" t="n">
+      <c r="S22" t="n">
         <v>0.1388681207392253</v>
       </c>
     </row>
@@ -1648,9 +1852,18 @@
         <v>0.5673792018732057</v>
       </c>
       <c r="O23" t="n">
+        <v>0.05250176225054493</v>
+      </c>
+      <c r="P23" t="n">
+        <v>0.2340072372899777</v>
+      </c>
+      <c r="Q23" t="n">
+        <v>4.45713109920513</v>
+      </c>
+      <c r="R23" t="n">
         <v>0.6192685873876558</v>
       </c>
-      <c r="P23" t="n">
+      <c r="S23" t="n">
         <v>0.1389388316395033</v>
       </c>
     </row>
@@ -1700,9 +1913,18 @@
         <v>0.5895111229784974</v>
       </c>
       <c r="O24" t="n">
+        <v>0.05414453527536292</v>
+      </c>
+      <c r="P24" t="n">
+        <v>0.2372876176292924</v>
+      </c>
+      <c r="Q24" t="n">
+        <v>4.382485073009095</v>
+      </c>
+      <c r="R24" t="n">
         <v>0.6172706023174594</v>
       </c>
-      <c r="P24" t="n">
+      <c r="S24" t="n">
         <v>0.1408494477526264</v>
       </c>
     </row>
@@ -1752,9 +1974,18 @@
         <v>0.5855730403102242</v>
       </c>
       <c r="O25" t="n">
+        <v>0.050177583335919</v>
+      </c>
+      <c r="P25" t="n">
+        <v>0.2308983900100808</v>
+      </c>
+      <c r="Q25" t="n">
+        <v>4.601624364097165</v>
+      </c>
+      <c r="R25" t="n">
         <v>0.5830142465914784</v>
       </c>
-      <c r="P25" t="n">
+      <c r="S25" t="n">
         <v>0.1266974877698139</v>
       </c>
     </row>
@@ -1804,9 +2035,18 @@
         <v>0.4913675343993383</v>
       </c>
       <c r="O26" t="n">
+        <v>0.04878472332253792</v>
+      </c>
+      <c r="P26" t="n">
+        <v>0.2459265020784911</v>
+      </c>
+      <c r="Q26" t="n">
+        <v>5.041055587269802</v>
+      </c>
+      <c r="R26" t="n">
         <v>0.6402340491920678</v>
       </c>
-      <c r="P26" t="n">
+      <c r="S26" t="n">
         <v>0.1270039653617099</v>
       </c>
     </row>
@@ -1856,9 +2096,18 @@
         <v>0.4409872813152139</v>
       </c>
       <c r="O27" t="n">
+        <v>0.04722609046233642</v>
+      </c>
+      <c r="P27" t="n">
+        <v>0.2498689886636276</v>
+      </c>
+      <c r="Q27" t="n">
+        <v>5.290909880903697</v>
+      </c>
+      <c r="R27" t="n">
         <v>0.6660367293530616</v>
       </c>
-      <c r="P27" t="n">
+      <c r="S27" t="n">
         <v>0.1258832118379044</v>
       </c>
     </row>
@@ -1908,9 +2157,18 @@
         <v>0.428275461066541</v>
       </c>
       <c r="O28" t="n">
+        <v>0.04104926478163028</v>
+      </c>
+      <c r="P28" t="n">
+        <v>0.2160415820788314</v>
+      </c>
+      <c r="Q28" t="n">
+        <v>5.26298298466751</v>
+      </c>
+      <c r="R28" t="n">
         <v>0.6237116327281061</v>
       </c>
-      <c r="P28" t="n">
+      <c r="S28" t="n">
         <v>0.1185091486225865</v>
       </c>
     </row>
@@ -1960,9 +2218,18 @@
         <v>0.6559926976097419</v>
       </c>
       <c r="O29" t="n">
+        <v>0.05088369998143091</v>
+      </c>
+      <c r="P29" t="n">
+        <v>0.2129486294356157</v>
+      </c>
+      <c r="Q29" t="n">
+        <v>4.185006780429243</v>
+      </c>
+      <c r="R29" t="n">
         <v>0.5406663408426609</v>
       </c>
-      <c r="P29" t="n">
+      <c r="S29" t="n">
         <v>0.1291912699809787</v>
       </c>
     </row>

</xml_diff>